<commit_message>
new changes in corejava
</commit_message>
<xml_diff>
--- a/collection framework.xlsx
+++ b/collection framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="336" windowWidth="20832" windowHeight="10260"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="20835" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
   <si>
     <t>Principal collection class</t>
   </si>
@@ -308,6 +308,10 @@
 with no duplicates and you don't care about order when you iterate through it.</t>
   </si>
   <si>
+    <t>A LinkedHashSet is an ordered version of HashSet that maintains a doubly-linked List across all elements. Use this class instead of HashSet when you care about the iteration order. When you iterate through a HashSet the
+order is unpredictable, while a LinkedHashSet lets you iterate through the elements in the order in which they were inserted.</t>
+  </si>
+  <si>
     <t>The TreeSet is one of two sorted collections (the other being TreeMap). It uses a Red-Black tree structure (but you knew that), and guarantees that the elements will be in ascending order, according to natural order. Optionally, you can construct a TreeSet with a constructor that lets you give the collection your own rules for what the order should be (rather than relying on the ordering defined by the elements' class) by using a Comparable or Comparator. As of Java 6, TreeSet implements NavigableSet.</t>
   </si>
   <si>
@@ -336,6 +340,17 @@
       </rPr>
       <t>When a collection is ordered, it means you can iterate through the collection in a specific (not-random) order.</t>
     </r>
+  </si>
+  <si>
+    <t>A LinkedList is ordered by index position, like ArrayList, except that the elements are doubly-linked to one another. This linkage gives you new methods (beyond what you get from the List interface) for adding and removing
+from the beginning or end, which makes it an easy choice for implementing a stack or queue. Keep in mind that a LinkedList may iterate more slowly than an ArrayList, but it's a good choice when you need fast insertion and deletion. 
+As of Java 5, the LinkedList class has been enhanced to implement the java.util.Queue interface. As
+such, it now supports the common queue methods: peek(), poll(), and offer().
+LinkedList by nature does not have "capacity", since it does not allocate memory to the items before the items are added to the list. 
+Each item in a LinkedList holds a pointer to the next in the list. But it is costly to have random access to the elements in the List. 
+You need to go through all the Elements in the list until you reach your destination.
+ArrayList is backed up by an array, so the initial capacity is the initial size of the array. 
+LinkedList has no need of that.</t>
   </si>
   <si>
     <t>Ordered by?</t>
@@ -394,52 +409,12 @@
  - compare(key, key); // type (and possibly null) check
 The above line is used to check the NULL and Type of Keys, But this line is not available in Java 6 TreeMap Class.</t>
   </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> doubly linked list </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>whose nodes contain three fields: an integer value, the link to the next node, and the link to the previous node.</t>
-    </r>
-  </si>
-  <si>
-    <t>A LinkedList is ordered by index position, like ArrayList, except that the elements are doubly-linked to one another. 
-This linkage enables adding and removing from the beginning or end, which makes it an easy choice for implementing a stack or queue. Keep in mind that a LinkedList may iterate more slowly than an ArrayList, but it's a good choice when you need fast insertion and deletion. 
-Operations that index into the list will traverse the list from the beginning or the end, whichever is closer to the specified index.
-As of Java 5, the LinkedList class has been enhanced to implement the java.util.Queue interface. As such, it now supports the common queue methods: peek(), poll(), and offer().
-LinkedList by nature does not have "capacity", since it does not allocate memory to the items before the items are added to the list. 
-Each item in a LinkedList holds a pointer to the next in the list. But it is costly to have random access to the elements in the List. 
-You need to go through all the Elements in the list until you reach your destination.
-ArrayList is backed up by an array, so the initial capacity is the initial size of the array. 
-LinkedList has no need of that.</t>
-  </si>
-  <si>
-    <t>A LinkedHashSet is an ordered version of HashSet that maintains a doubly-linked List across all elements. Use this class instead of HashSet when you care about the iteration order. When you iterate through a HashSet the order is unpredictable, while a LinkedHashSet lets you iterate through the elements in the order in which they were inserted.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,13 +678,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -717,54 +734,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -796,13 +795,20 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -881,7 +887,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -916,7 +921,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1092,49 +1096,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N26" sqref="N26"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="59.5546875" style="30" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="70.88671875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="70.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="26.88671875" style="4"/>
+    <col min="11" max="11" width="10.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="26.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C1" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-    </row>
-    <row r="2" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C2" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-    </row>
-    <row r="3" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15">
+      <c r="C1" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+    </row>
+    <row r="3" spans="1:13" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1166,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>3</v>
@@ -1175,14 +1172,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:13" ht="76.5">
+      <c r="A4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="35" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1207,7 +1204,7 @@
         <v>5</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>6</v>
@@ -1216,10 +1213,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="105.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="46"/>
+    <row r="5" spans="1:13" ht="63.75">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1242,70 +1239,70 @@
         <v>5</v>
       </c>
       <c r="K5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="36" t="s">
+      <c r="G6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="208.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37" t="s">
+      <c r="I6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="208.5" customHeight="1">
+      <c r="A7" s="39"/>
+      <c r="B7" s="39" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-    </row>
-    <row r="8" spans="1:13" ht="145.19999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+    </row>
+    <row r="8" spans="1:13" ht="114.75">
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="11" t="s">
         <v>38</v>
       </c>
@@ -1313,7 +1310,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>14</v>
@@ -1331,7 +1328,7 @@
         <v>5</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>6</v>
@@ -1340,12 +1337,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
-      <c r="B9" s="39" t="s">
+    <row r="9" spans="1:13" ht="70.5" customHeight="1">
+      <c r="A9" s="39"/>
+      <c r="B9" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="32" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -1379,15 +1376,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="45"/>
+    <row r="10" spans="1:13" ht="78" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>14</v>
@@ -1405,7 +1402,7 @@
         <v>5</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L10" s="18" t="s">
         <v>6</v>
@@ -1414,17 +1411,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+    <row r="11" spans="1:13" ht="100.5" customHeight="1">
+      <c r="A11" s="39"/>
       <c r="B11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="33"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>14</v>
@@ -1436,13 +1433,13 @@
         <v>14</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>5</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L11" s="19" t="s">
         <v>5</v>
@@ -1451,8 +1448,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
+    <row r="12" spans="1:13">
+      <c r="A12" s="39"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
@@ -1466,8 +1463,8 @@
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
+    <row r="13" spans="1:13">
+      <c r="A13" s="39"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
@@ -1481,19 +1478,19 @@
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
     </row>
-    <row r="14" spans="1:13" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
-      <c r="B14" s="41" t="s">
+    <row r="14" spans="1:13" ht="81.75" customHeight="1">
+      <c r="A14" s="39"/>
+      <c r="B14" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F14" s="26" t="s">
         <v>6</v>
@@ -1520,15 +1517,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="32"/>
+    <row r="15" spans="1:13" ht="60" customHeight="1">
+      <c r="A15" s="39"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="25" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F15" s="26" t="s">
         <v>6</v>
@@ -1536,9 +1533,7 @@
       <c r="G15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="26" t="s">
-        <v>5</v>
-      </c>
+      <c r="H15" s="26"/>
       <c r="I15" s="26" t="s">
         <v>5</v>
       </c>
@@ -1546,7 +1541,7 @@
         <v>5</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L15" s="26" t="s">
         <v>6</v>
@@ -1555,15 +1550,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="32"/>
+    <row r="16" spans="1:13" ht="120" customHeight="1">
+      <c r="A16" s="39"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="25" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F16" s="26" t="s">
         <v>6</v>
@@ -1590,17 +1585,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="256.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
+    <row r="17" spans="1:13" ht="256.5" customHeight="1">
+      <c r="A17" s="39"/>
       <c r="B17" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="33"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="25" t="s">
         <v>32</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F17" s="26" t="s">
         <v>6</v>
@@ -1618,7 +1613,7 @@
         <v>5</v>
       </c>
       <c r="K17" s="27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L17" s="27" t="s">
         <v>5</v>
@@ -1627,23 +1622,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13">
       <c r="B20" s="29"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="D22" s="29"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="D23" s="29"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="D24" s="29"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="D25" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
@@ -1652,28 +1659,15 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:M1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",F1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1683,24 +1677,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new changes for carejava
</commit_message>
<xml_diff>
--- a/collection framework.xlsx
+++ b/collection framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="20835" windowHeight="10260"/>
+    <workbookView xWindow="480" yWindow="336" windowWidth="20832" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -245,12 +245,6 @@
     </r>
   </si>
   <si>
-    <t>A Map cares about unique identifiers. You map a unique key (the ID) to a specific value, where both the key and the value are, of course, objects. 
-The Map implementations let you do things like search for a
-value based on the key, ask for a collection of just the values, or ask for a collection of just the keys. 
-Like Sets, Maps rely on the equals() method to determine whether two keys are the same or different.</t>
-  </si>
-  <si>
     <t>A List cares about the index. 
 The one thing that List has that non-lists don't have is a set of methods related to the index. 
 Those key methods include things like get(int index), indexOf(Object o), add(int index, Object obj), and so on. 
@@ -304,14 +298,6 @@
 </t>
   </si>
   <si>
-    <t>A HashSet is an unsorted, unordered Set. It uses the hashcode of the object being inserted, so the more efficient your hashCode() implementation the better access performance you'll get. Use this class when you want a collection
-with no duplicates and you don't care about order when you iterate through it.</t>
-  </si>
-  <si>
-    <t>A LinkedHashSet is an ordered version of HashSet that maintains a doubly-linked List across all elements. Use this class instead of HashSet when you care about the iteration order. When you iterate through a HashSet the
-order is unpredictable, while a LinkedHashSet lets you iterate through the elements in the order in which they were inserted.</t>
-  </si>
-  <si>
     <t>The TreeSet is one of two sorted collections (the other being TreeMap). It uses a Red-Black tree structure (but you knew that), and guarantees that the elements will be in ascending order, according to natural order. Optionally, you can construct a TreeSet with a constructor that lets you give the collection your own rules for what the order should be (rather than relying on the ordering defined by the elements' class) by using a Comparable or Comparator. As of Java 6, TreeSet implements NavigableSet.</t>
   </si>
   <si>
@@ -342,10 +328,38 @@
     </r>
   </si>
   <si>
+    <t>Ordered by?</t>
+  </si>
+  <si>
+    <t>By Index</t>
+  </si>
+  <si>
+    <t>natural ordering, or by a Comparator provided at queue construction time</t>
+  </si>
+  <si>
+    <t>insertion-order</t>
+  </si>
+  <si>
+    <t> natural ordering, or by a Comparator provided at set creation time</t>
+  </si>
+  <si>
+    <t>Yes
+(Yes, you can. But you will have to provide your own Comparator to handle the case when null is compared to any other contents of your set. With natural ordering applied, Java objects do not know how to compare themselves to null. Inversely, null doesn't know how to compare itself with any object as you cannot call null.compareTo(object).</t>
+  </si>
+  <si>
+    <t>natural ordering of its keys, or by a Comparator provided at map creation time</t>
+  </si>
+  <si>
+    <t>You can probably guess by now that a TreeMap is a sorted Map. And you already know that by default, this means "sorted by the natural order of the elements." Like TreeSet, TreeMap lets you define a custom sort order (via a Comparable or Comparator) when you construct a TreeMap, that specifies how the elements should be compared to one another when they're being ordered. As of Java 6, TreeMap implements NavigableMap.
+JAVA6 -  Insert an Entry with null key in empty TreeMap is allowed. But after inserting this entry if we are trying to insert any other Entry we will get NullPointerException.(i.e TreeMap allows Null key only once if it is an empty TreeMap)
+JAVA7 - Here TreeMap shouldn’t allow NULL keys at any situation. If we are trying to insert the NULL keys we will get NullPointerException.
+ - compare(key, key); // type (and possibly null) check
+The above line is used to check the NULL and Type of Keys, But this line is not available in Java 6 TreeMap Class.</t>
+  </si>
+  <si>
     <t>A LinkedList is ordered by index position, like ArrayList, except that the elements are doubly-linked to one another. This linkage gives you new methods (beyond what you get from the List interface) for adding and removing
 from the beginning or end, which makes it an easy choice for implementing a stack or queue. Keep in mind that a LinkedList may iterate more slowly than an ArrayList, but it's a good choice when you need fast insertion and deletion. 
-As of Java 5, the LinkedList class has been enhanced to implement the java.util.Queue interface. As
-such, it now supports the common queue methods: peek(), poll(), and offer().
+As of Java 5, the LinkedList class has been enhanced to implement the java.util.Queue interface. As such, it now supports the common queue methods: peek(), poll(), and offer().
 LinkedList by nature does not have "capacity", since it does not allocate memory to the items before the items are added to the list. 
 Each item in a LinkedList holds a pointer to the next in the list. But it is costly to have random access to the elements in the List. 
 You need to go through all the Elements in the list until you reach your destination.
@@ -353,18 +367,8 @@
 LinkedList has no need of that.</t>
   </si>
   <si>
-    <t>Ordered by?</t>
-  </si>
-  <si>
-    <t>By Index</t>
-  </si>
-  <si>
-    <t>natural ordering, or by a Comparator provided at queue construction time</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This class is new with Java 5. Since the LinkedList class has been enhanced to implement the Queue interface, basic queues can be handled with a LinkedList. The purpose of a PriorityQueue is to create a "priority-in, priority out"
-queue as opposed to a typical FIFO queue. A PriorityQueue's elements are ordered either by natural ordering (in which case the elements that are sorted first will be accessed first) or according to a Comparator. In either case, the elements' ordering represents their relative priority.
+    <r>
+      <t xml:space="preserve">This class is new with Java 5. Since the LinkedList class has been enhanced to implement the Queue interface, basic queues can be handled with a LinkedList. The purpose of a PriorityQueue is to create a "priority-in, priority out" queue as opposed to a typical FIFO queue. A PriorityQueue's elements are ordered either by natural ordering (in which case the elements that are sorted first will be accessed first) or according to a Comparator. In either case, the elements' ordering represents their relative priority.
 </t>
     </r>
     <r>
@@ -381,40 +385,27 @@
     </r>
   </si>
   <si>
-    <t>insertion-order</t>
-  </si>
-  <si>
-    <t> natural ordering, or by a Comparator provided at set creation time</t>
-  </si>
-  <si>
-    <t>Yes
-(Yes, you can. But you will have to provide your own Comparator to handle the case when null is compared to any other contents of your set. With natural ordering applied, Java objects do not know how to compare themselves to null. Inversely, null doesn't know how to compare itself with any object as you cannot call null.compareTo(object).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Like its Set counterpart, LinkedHashSet, the LinkedHash-Map collection maintains insertion order (or, optionally, access order). Although it will be somewhat slower than HashMap for adding and removing elements, you can
-expect faster iteration with a LinkedHashMap.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Like Vector, Hashtable has existed from prehistoric Java times. For fun, don't forget to note the naming inconsistency: HashMap vs. Hashtable. Where's the capitalization of t? Oh well, you won't be expected to spell it. Anyway, just as Vector is a synchronized counterpart to the sleeker, more modern ArrayList, Hashtable is the synchronized counterpart to HashMap. Remember that you don't synchronize a class, so when we say that Vector and Hashtable are synchronized, we just mean that the key methods of the class are synchronized. Another difference, though, is that while HashMap lets you have null values as well as one null key, a Hashtable doesn't let you have anything that's null.
-</t>
-  </si>
-  <si>
-    <t>natural ordering of its keys, or by a Comparator provided at map creation time</t>
-  </si>
-  <si>
-    <t>You can probably guess by now that a TreeMap is a sorted Map. And you already know that by default, this means "sorted by the natural order of the elements." Like TreeSet, TreeMap lets you define a custom sort order (via a Comparable or Comparator) when you construct a TreeMap, that specifies how the elements should be compared to one another when they're being ordered. As of Java 6, TreeMap implements NavigableMap.
-JAVA6 -  Insert an Entry with null key in empty TreeMap is allowed. But after inserting this entry if we are trying to insert any other Entry we will get NullPointerException.(i.e TreeMap allows Null key only once if it is an empty TreeMap)
-JAVA7 - Here TreeMap shouldn’t allow NULL keys at any situation. If we are trying to insert the NULL keys we will get NullPointerException.
- - compare(key, key); // type (and possibly null) check
-The above line is used to check the NULL and Type of Keys, But this line is not available in Java 6 TreeMap Class.</t>
+    <t>A HashSet is an unsorted, unordered Set. It uses the hashcode of the object being inserted, so the more efficient your hashCode() implementation the better access performance you'll get. Use this class when you want a collection with no duplicates and you don't care about order when you iterate through it.</t>
+  </si>
+  <si>
+    <t>A LinkedHashSet is an ordered version of HashSet that maintains a doubly-linked List across all elements. Use this class instead of HashSet when you care about the iteration order. When you iterate through a HashSet the order is unpredictable, while a LinkedHashSet lets you iterate through the elements in the order in which they were inserted.</t>
+  </si>
+  <si>
+    <t>A Map cares about unique identifiers. You map a unique key (the ID) to a specific value, where both the key and the value are, of course, objects. 
+The Map implementations let you do things like search for a value based on the key, ask for a collection of just the values, or ask for a collection of just the keys. Like Sets, Maps rely on the equals() method to determine whether two keys are the same or different.</t>
+  </si>
+  <si>
+    <t>Like Vector, Hashtable has existed from prehistoric Java times. For fun, don't forget to note the naming inconsistency: HashMap vs. Hashtable. Where's the capitalization of t? Oh well, you won't be expected to spell it. Anyway, just as Vector is a synchronized counterpart to the sleeker, more modern ArrayList, Hashtable is the synchronized counterpart to HashMap. Remember that you don't synchronize a class, so when we say that Vector and Hashtable are synchronized, we just mean that the key methods of the class are synchronized. Another difference, though, is that while HashMap lets you have null values as well as one null key, a Hashtable doesn't let you have anything that's null.</t>
+  </si>
+  <si>
+    <t>Like its Set counterpart, LinkedHashSet, the LinkedHash-Map collection maintains insertion order (or, optionally, access order). Although it will be somewhat slower than HashMap for adding and removing elements, you can expect faster iteration with a LinkedHashMap.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,31 +730,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -795,20 +762,13 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -887,6 +847,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -921,6 +882,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1096,42 +1058,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="26.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="59.5703125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="70.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="59.5546875" style="30" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="70.88671875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" style="4" customWidth="1"/>
     <col min="10" max="10" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="26.85546875" style="4"/>
+    <col min="11" max="11" width="10.88671875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="26.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15">
+    <row r="1" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C1" s="48" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
     </row>
-    <row r="3" spans="1:13" ht="25.5">
+    <row r="3" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1125,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>3</v>
@@ -1172,7 +1134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="76.5">
+    <row r="4" spans="1:13" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>8</v>
       </c>
@@ -1180,13 +1142,13 @@
         <v>16</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>14</v>
@@ -1204,7 +1166,7 @@
         <v>5</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>6</v>
@@ -1213,7 +1175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="63.75">
+    <row r="5" spans="1:13" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A5" s="39"/>
       <c r="B5" s="40"/>
       <c r="C5" s="35"/>
@@ -1221,7 +1183,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>14</v>
@@ -1239,7 +1201,7 @@
         <v>5</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>6</v>
@@ -1248,7 +1210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="39"/>
       <c r="B6" s="40"/>
       <c r="C6" s="35"/>
@@ -1256,7 +1218,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F6" s="31" t="s">
         <v>14</v>
@@ -1274,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="K6" s="31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L6" s="31" t="s">
         <v>6</v>
@@ -1283,7 +1245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="208.5" customHeight="1">
+    <row r="7" spans="1:13" ht="208.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39"/>
       <c r="B7" s="39" t="s">
         <v>17</v>
@@ -1300,17 +1262,17 @@
       <c r="L7" s="31"/>
       <c r="M7" s="31"/>
     </row>
-    <row r="8" spans="1:13" ht="114.75">
+    <row r="8" spans="1:13" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>14</v>
@@ -1328,7 +1290,7 @@
         <v>5</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>6</v>
@@ -1337,19 +1299,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="70.5" customHeight="1">
+    <row r="9" spans="1:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="39"/>
       <c r="B9" s="41" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>14</v>
@@ -1376,7 +1338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="78" customHeight="1">
+    <row r="10" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="39"/>
       <c r="B10" s="42"/>
       <c r="C10" s="33"/>
@@ -1384,7 +1346,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>14</v>
@@ -1402,7 +1364,7 @@
         <v>5</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L10" s="18" t="s">
         <v>6</v>
@@ -1411,7 +1373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="100.5" customHeight="1">
+    <row r="11" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="39"/>
       <c r="B11" s="20" t="s">
         <v>18</v>
@@ -1421,7 +1383,7 @@
         <v>28</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>14</v>
@@ -1433,13 +1395,13 @@
         <v>14</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>5</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L11" s="19" t="s">
         <v>5</v>
@@ -1448,7 +1410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="39"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
@@ -1463,7 +1425,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="39"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
@@ -1478,19 +1440,19 @@
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
     </row>
-    <row r="14" spans="1:13" ht="81.75" customHeight="1">
+    <row r="14" spans="1:13" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="39"/>
       <c r="B14" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" s="26" t="s">
         <v>6</v>
@@ -1517,7 +1479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="60" customHeight="1">
+    <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="39"/>
       <c r="B15" s="44"/>
       <c r="C15" s="47"/>
@@ -1525,7 +1487,7 @@
         <v>30</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F15" s="26" t="s">
         <v>6</v>
@@ -1541,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L15" s="26" t="s">
         <v>6</v>
@@ -1550,7 +1512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="120" customHeight="1">
+    <row r="16" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="39"/>
       <c r="B16" s="45"/>
       <c r="C16" s="47"/>
@@ -1558,7 +1520,7 @@
         <v>31</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F16" s="26" t="s">
         <v>6</v>
@@ -1585,7 +1547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="256.5" customHeight="1">
+    <row r="17" spans="1:13" ht="256.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39"/>
       <c r="B17" s="28" t="s">
         <v>21</v>
@@ -1595,7 +1557,7 @@
         <v>32</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F17" s="26" t="s">
         <v>6</v>
@@ -1613,7 +1575,7 @@
         <v>5</v>
       </c>
       <c r="K17" s="27" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="L17" s="27" t="s">
         <v>5</v>
@@ -1622,19 +1584,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B20" s="29"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D22" s="29"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D23" s="29"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D24" s="29"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D25" s="29"/>
     </row>
   </sheetData>
@@ -1644,13 +1606,13 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="F6:F7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
@@ -1661,13 +1623,13 @@
     <mergeCell ref="K6:K7"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:M1048576">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",F1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1677,24 +1639,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>